<commit_message>
text with actual and predict values from new models
</commit_message>
<xml_diff>
--- a/Topic-Modeling-SIMS-v1.xlsx
+++ b/Topic-Modeling-SIMS-v1.xlsx
@@ -1,20 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
-  </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="96">
   <si>
     <t>Broad Category</t>
   </si>
@@ -175,34 +172,368 @@
     <t>Environmental disaster</t>
   </si>
   <si>
-    <t>কনক</t>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>কনকনে শীতে বিপর্যস্ত উত্তরাঞ্চলের জনজীবন</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>রাজধানীসহ দেশের বিভিন্ন স্থানে ভূমিকম্প অনুভূত হয়েছে</t>
+    </r>
+  </si>
+  <si>
+    <t>Cyber Crime</t>
+  </si>
+  <si>
+    <t>Hacking</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>নারী সেজে ইমো অ্যাকাউন্ট হ্যাকিং, যুবকের পাঁচ বছরের কারাদণ্ড</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>ওটিপি পাঠিয়ে ব্যাংক অ্যাকাউন্ট হ্যাকিং, সুরক্ষিত থাকতে যা করবেন</t>
+    </r>
+  </si>
+  <si>
+    <t>Scam/Fraud</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>ফেসবুক, হোয়াটসঅ্যাপ, টেলিগ্রামে বাড়ছে ‘পিগ বুচারিং’ প্রতারণা, নিরাপদ থাকবেন যেভাবে</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>ডেটিং অ্যাপে প্রতারণা থেকে নিরাপদ থাকবেন যেভাবে</t>
+    </r>
+  </si>
+  <si>
+    <t>Sextortion</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>যৌনতা নিয়ে খোলামেলা আলাপ করে জনপ্রিয়, কে এই ৬২ বছর বয়সী ইউটিউবার</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>সোনার বিনিময়ে এই খনিতে বিক্রি হয় যৌনতা</t>
+    </r>
+  </si>
+  <si>
+    <t>Data breaches</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>২৬০০ কোটি ডেটা ফাঁস, বড় ধরনের সাইবার হামলার শঙ্কা</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>এনআইডির তথ্য বিক্রি: ৪৬ ধরনের ব্যক্তিগত তথ্য ফাঁস</t>
+    </r>
+  </si>
+  <si>
+    <t>Cyberterrorism</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>সাইবার সুরক্ষা অধ্যাদেশ: সরকারের জবাবদিহির বিষয়টি স্পষ্ট নয়</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>ক্রোমের একাধিক এক্সটেনশনে সাইবার হামলা, ব্যবহারকারীদের তথ্য চুরির আশঙ্কা</t>
+    </r>
+  </si>
+  <si>
+    <t>Online Harassment and Cyberbullying</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>ফেসবুকে পোস্ট শেয়ার করায় সাইবার নিরাপত্তা আইনে মামলা, তরুণ গ্রেপ্তার</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>অপব্যবহারের ঝুঁকি রয়েই গেল সাইবার সুরক্ষা অধ্যাদেশে</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dark web activity</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>ডার্ক ওয়েবের হাতছানি পড়ুয়াদের সামনে, অনলাইনে ক্লাস নিয়ে আরও সতর্ক হতে পরামর্শ বিশেষজ্ঞের</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>ডার্কওয়েবে রমরমা মাদকের কারবার, বাড়ছে উদ্বেগ</t>
+    </r>
+  </si>
+  <si>
+    <t>Cryptocurrency</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>প্রায় ৩১ কোটি ডলারের বিটকয়েন চুরি করা হ্যাকার দলের পরিচয় শনাক্ত</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>রেকর্ডের পর রেকর্ড গড়ার পর কমেছে বিটকয়েনের দাম</t>
+    </r>
+  </si>
+  <si>
+    <t>Misinformation / Disinformation (includes provocative news, false news, rumor, misleading)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>সামাজিক যোগাযোগমাধ্যমে ভুয়া ভিডিওর মাধ্যমে ছড়াচ্ছে স্বাস্থ্যবিষয়ক বিপজ্জনক তথ্য</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>ভুয়া তথ্য দিয়ে ই-পাসপোর্টও পান আজিজের দুই ভাই</t>
+    </r>
+  </si>
+  <si>
+    <t>Religious Dispute</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>সুদ-ঘুষ নিয়ে বয়ান করায় ইমামকে চাকরি ছাড়তে বললেন সভাপতি</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>বান্দরবানে ত্রিপুরা খ্রিস্টান সম্প্রদায়ের ১৭টি বসতঘরে আগুন</t>
+    </r>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>মিডিয়া পলিটিকস নিয়ে বিস্ফোরক দীঘি</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>রাজনৈতিক অস্থিরতার প্রভাব বিনোদন অঙ্গনে</t>
+    </r>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>চ্যাম্পিয়নস ট্রফিতেও কামিন্সের খেলা নিয়ে সংশয়, কারণ...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>আফগানদের টুর্নামেন্ট-দর্শন: যে দেশে খেলা, সে দেশ থেকে ‘মেন্টর’</t>
+    </r>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>কোক খেলে মানুষের আয়ু কমে ১২ মিনিট, অন্যান্য ফাস্ট ফুডে কত</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>টিফ ২০২৪: মূল প্রতিযোগিতার বাইরের অন্যান্য দিক</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="7">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="13.0"/>
       <color rgb="FF374151"/>
       <name val="__Inter_d65c78"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
       <color rgb="FF374151"/>
       <name val="__Inter_d65c78"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FFD6D6DD"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FFD6D6DD"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -210,22 +541,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf4f4f5"/>
+        <fgColor rgb="FFF4F4F5"/>
+        <bgColor rgb="FFF4F4F5"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -239,46 +565,57 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="8">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -305,82 +642,22 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -392,184 +669,156 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
-            </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" style="3" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="41.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="69.7192857142857" customWidth="1" bestFit="1"/>
+    <col customWidth="1" min="1" max="1" width="19.0"/>
+    <col customWidth="1" min="2" max="2" width="41.13"/>
+    <col customWidth="1" min="3" max="3" width="69.75"/>
+    <col customWidth="1" min="4" max="4" width="21.88"/>
+    <col customWidth="1" min="5" max="5" width="39.25"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -591,7 +840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -602,7 +851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -613,7 +862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -624,7 +873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -635,7 +884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -646,7 +895,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -657,7 +906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+    <row r="9">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -668,7 +917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+    <row r="10">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -679,7 +928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
+    <row r="11">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -690,7 +939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+    <row r="12">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -701,7 +950,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+    <row r="13">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -712,7 +961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+    <row r="14">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -723,7 +972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+    <row r="15">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -734,7 +983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+    <row r="16">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -745,7 +994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+    <row r="17">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -756,7 +1005,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
+    <row r="18">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -767,7 +1016,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
+    <row r="19">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -778,7 +1027,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
+    <row r="20">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -789,7 +1038,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
+    <row r="21">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -800,7 +1049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
+    <row r="22">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -811,7 +1060,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row r="23">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -822,7 +1071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row r="24">
       <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
@@ -833,7 +1082,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row r="25">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
@@ -844,7 +1093,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row r="26">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -855,7 +1104,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row r="27">
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
@@ -866,7 +1115,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row r="28">
       <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
@@ -877,7 +1126,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row r="29">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -888,7 +1137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row r="30">
       <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
@@ -899,7 +1148,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row r="31">
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
@@ -910,18 +1159,350 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row r="32">
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>53</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" ht="16.5" customHeight="1">
+      <c r="A54" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A59">
+      <formula1>"Politics,Crime,Corruption,Accident,Cyber Crime,Entertainment,Others"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C32"/>
+    <hyperlink r:id="rId2" ref="C33"/>
+    <hyperlink r:id="rId3" ref="C34"/>
+    <hyperlink r:id="rId4" ref="C35"/>
+    <hyperlink r:id="rId5" ref="C36"/>
+    <hyperlink r:id="rId6" ref="C37"/>
+    <hyperlink r:id="rId7" ref="C38"/>
+    <hyperlink r:id="rId8" ref="C39"/>
+    <hyperlink r:id="rId9" ref="C40"/>
+    <hyperlink r:id="rId10" ref="C41"/>
+    <hyperlink r:id="rId11" ref="C42"/>
+    <hyperlink r:id="rId12" ref="C43"/>
+    <hyperlink r:id="rId13" ref="C44"/>
+    <hyperlink r:id="rId14" ref="C45"/>
+    <hyperlink r:id="rId15" ref="C46"/>
+    <hyperlink r:id="rId16" ref="C47"/>
+    <hyperlink r:id="rId17" ref="C48"/>
+    <hyperlink r:id="rId18" ref="C49"/>
+    <hyperlink r:id="rId19" ref="C50"/>
+    <hyperlink r:id="rId20" ref="C51"/>
+    <hyperlink r:id="rId21" ref="C52"/>
+    <hyperlink r:id="rId22" ref="C53"/>
+    <hyperlink r:id="rId23" ref="C54"/>
+    <hyperlink r:id="rId24" ref="C55"/>
+    <hyperlink r:id="rId25" ref="C56"/>
+    <hyperlink r:id="rId26" ref="C57"/>
+    <hyperlink r:id="rId27" ref="C58"/>
+    <hyperlink r:id="rId28" ref="C59"/>
+  </hyperlinks>
+  <drawing r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>